<commit_message>
Add a feature to add a new stock to the inventory
</commit_message>
<xml_diff>
--- a/coffee_stock_inventory.xlsx
+++ b/coffee_stock_inventory.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,13 +24,45 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -45,8 +77,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,270 +449,271 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.5546875" customWidth="1" min="1" max="1"/>
-    <col width="16.109375" customWidth="1" min="2" max="2"/>
-    <col width="15.6640625" customWidth="1" min="3" max="3"/>
-    <col width="12.6640625" customWidth="1" min="4" max="4"/>
-    <col width="14.6640625" customWidth="1" min="5" max="5"/>
+    <col width="17.5546875" customWidth="1" style="1" min="1" max="1"/>
+    <col width="16.109375" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15.6640625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="12.6640625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="14.6640625" customWidth="1" style="1" min="5" max="5"/>
+    <col width="8.88671875" customWidth="1" style="1" min="6" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Coffee Pack</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Price (€)</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>13.00</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
         <is>
           <t>13.00</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
         <is>
           <t>37.00</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
         <is>
           <t>37.00</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>2.5kg</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
         <is>
           <t>85.00</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -701,81 +739,81 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="5" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="5" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
         <is>
           <t>15.70</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -805,378 +843,378 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="4" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="4" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
+      <c r="C17" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="4" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
+      <c r="C18" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
         <is>
           <t>57.00</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="4" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
+      <c r="C19" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="inlineStr">
         <is>
           <t>57.00</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="4" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="5" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
         <is>
           <t>14.00</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="4" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="inlineStr">
         <is>
           <t>14.00</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="4" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
+      <c r="C24" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="inlineStr">
         <is>
           <t>24.60</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="4" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
+      <c r="C25" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="inlineStr">
         <is>
           <t>24.60</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="4" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
+      <c r="C26" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="inlineStr">
         <is>
           <t>45.00</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="4" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
+      <c r="C27" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D27" s="4" t="inlineStr">
         <is>
           <t>45.00</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="4" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
+      <c r="C28" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D28" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="E28" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="5" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="E29" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="5" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
+      <c r="B30" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="inlineStr">
         <is>
           <t>15.70</t>
         </is>
       </c>
-      <c r="E30" t="n">
-        <v>1</v>
+      <c r="E30" s="5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -1205,477 +1243,477 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="4" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D32" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="E32" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="4" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
+      <c r="C33" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D33" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="E33" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="4" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
+      <c r="C34" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
         <is>
           <t>57.00</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="4" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
+      <c r="C35" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D35" s="4" t="inlineStr">
         <is>
           <t>57.00</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="E35" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="5" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D36" s="5" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="E36" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="4" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
+      <c r="C37" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D37" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="5" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
+      <c r="B38" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D38" s="5" t="inlineStr">
         <is>
           <t>13.00</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="5" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
+      <c r="B39" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D39" s="5" t="inlineStr">
         <is>
           <t>13.00</t>
         </is>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="4" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
+      <c r="C40" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D40" s="4" t="inlineStr">
         <is>
           <t>24.60</t>
         </is>
       </c>
-      <c r="E40" t="n">
+      <c r="E40" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="4" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
         <is>
           <t>24.60</t>
         </is>
       </c>
-      <c r="E41" t="n">
+      <c r="E41" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="4" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
+      <c r="C42" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
         <is>
           <t>45.00</t>
         </is>
       </c>
-      <c r="E42" t="n">
+      <c r="E42" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="4" t="inlineStr">
         <is>
           <t>Yetu Tamu</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="inlineStr">
         <is>
           <t>45.00</t>
         </is>
       </c>
-      <c r="E43" t="n">
+      <c r="E43" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="4" t="inlineStr">
         <is>
           <t>House of Signatures</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C44" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D44" s="4" t="inlineStr">
         <is>
           <t>16.00</t>
         </is>
       </c>
-      <c r="E44" t="n">
+      <c r="E44" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="4" t="inlineStr">
         <is>
           <t>House of Signatures</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D45" s="4" t="inlineStr">
         <is>
           <t>16.00</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="E45" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="4" t="inlineStr">
         <is>
           <t>House of Signatures</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
+      <c r="C46" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D46" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E46" t="n">
+      <c r="E46" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="4" t="inlineStr">
         <is>
           <t>House of Signatures</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
+      <c r="C47" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D47" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E47" t="n">
+      <c r="E47" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="4" t="inlineStr">
         <is>
           <t>House of Signatures</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
+      <c r="C48" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D48" s="4" t="inlineStr">
         <is>
           <t>60.00</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="E48" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="4" t="inlineStr">
         <is>
           <t>House of Signatures</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
+      <c r="C49" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D49" s="4" t="inlineStr">
         <is>
           <t>60.00</t>
         </is>
       </c>
-      <c r="E49" t="n">
+      <c r="E49" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="5" t="inlineStr">
         <is>
           <t>Kivu D.R. Congo</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="5" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
+      <c r="C50" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D50" s="5" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E50" t="n">
+      <c r="E50" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1730,252 +1768,252 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="5" t="inlineStr">
         <is>
           <t>Kivu D.R. Congo</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
+      <c r="B53" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C53" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D53" s="5" t="inlineStr">
         <is>
           <t>15.70</t>
         </is>
       </c>
-      <c r="E53" t="n">
+      <c r="E53" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="4" t="inlineStr">
         <is>
           <t>Kivu D.R. Congo</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
+      <c r="C54" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D54" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E54" t="n">
+      <c r="E54" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="4" t="inlineStr">
         <is>
           <t>Kivu D.R. Congo</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
+      <c r="C55" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="E55" t="n">
+      <c r="E55" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="4" t="inlineStr">
         <is>
           <t>Kivu D.R. Congo</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B56" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D56" s="4" t="inlineStr">
         <is>
           <t>57.00</t>
         </is>
       </c>
-      <c r="E56" t="n">
+      <c r="E56" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="4" t="inlineStr">
         <is>
           <t>Kivu D.R. Congo</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B57" s="4" t="inlineStr">
         <is>
           <t>1kg</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
+      <c r="C57" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D57" s="4" t="inlineStr">
         <is>
           <t>57.00</t>
         </is>
       </c>
-      <c r="E57" t="n">
+      <c r="E57" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="5" t="inlineStr">
         <is>
           <t>Glory to Ukraine</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
+      <c r="B58" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C58" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D58" s="5" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E58" t="n">
+      <c r="E58" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="5" t="inlineStr">
         <is>
           <t>Glory to Ukraine</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
+      <c r="B59" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C59" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D59" s="5" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E59" t="n">
+      <c r="E59" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="4" t="inlineStr">
         <is>
           <t>Rebuild Ukraine</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C60" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D60" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E60" t="n">
+      <c r="E60" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="4" t="inlineStr">
         <is>
           <t>Rebuild Ukraine</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
+      <c r="B61" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C61" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D61" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E61" t="n">
+      <c r="E61" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="5" t="inlineStr">
         <is>
           <t>Coffee sets</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B62" s="5" t="inlineStr">
         <is>
           <t>400g</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
+      <c r="C62" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D62" s="5" t="inlineStr">
         <is>
           <t>30.00</t>
         </is>
       </c>
-      <c r="E62" t="n">
+      <c r="E62" s="5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2005,252 +2043,252 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="4" t="inlineStr">
         <is>
           <t>Aciu</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D64" s="4" t="inlineStr">
         <is>
           <t>15.50</t>
         </is>
       </c>
-      <c r="E64" t="n">
+      <c r="E64" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="4" t="inlineStr">
         <is>
           <t>Aciu</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D65" s="4" t="inlineStr">
         <is>
           <t>15.50</t>
         </is>
       </c>
-      <c r="E65" t="n">
+      <c r="E65" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="4" t="inlineStr">
         <is>
           <t>Love Birds</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D66" s="4" t="inlineStr">
         <is>
           <t>15.50</t>
         </is>
       </c>
-      <c r="E66" t="n">
+      <c r="E66" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="4" t="inlineStr">
         <is>
           <t>Love Birds</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D67" s="4" t="inlineStr">
         <is>
           <t>15.50</t>
         </is>
       </c>
-      <c r="E67" t="n">
+      <c r="E67" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" s="4" t="inlineStr">
         <is>
           <t>As ir Tu</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D68" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E68" t="n">
+      <c r="E68" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="4" t="inlineStr">
         <is>
           <t>As ir Tu</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C69" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D69" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E69" t="n">
+      <c r="E69" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="4" t="inlineStr">
         <is>
           <t>Decafe Nyeri</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C70" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D70" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E70" t="n">
+      <c r="E70" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="4" t="inlineStr">
         <is>
           <t>Decafe Nyeri</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
+      <c r="B71" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C71" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D71" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E71" t="n">
+      <c r="E71" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
+      <c r="A72" s="4" t="inlineStr">
         <is>
           <t>Upendo Africa</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B72" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
+      <c r="C72" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D72" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E72" t="n">
+      <c r="E72" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" s="4" t="inlineStr">
         <is>
           <t>Upendo Africa</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B73" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
+      <c r="C73" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D73" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E73" t="n">
+      <c r="E73" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2276,131 +2314,131 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="A75" s="5" t="inlineStr">
         <is>
           <t>Upendo Africa</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
+      <c r="B75" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C75" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D75" s="5" t="inlineStr">
         <is>
           <t>15.70</t>
         </is>
       </c>
-      <c r="E75" t="n">
+      <c r="E75" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
+      <c r="A76" s="4" t="inlineStr">
         <is>
           <t>Warmest Greetings</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
+      <c r="B76" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C76" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D76" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E76" t="n">
+      <c r="E76" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
+      <c r="A77" s="5" t="inlineStr">
         <is>
           <t>Warmest Greetings</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
+      <c r="B77" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C77" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D77" s="5" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E77" t="n">
+      <c r="E77" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" s="4" t="inlineStr">
         <is>
           <t>Nyeri</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B78" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
+      <c r="C78" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D78" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E78" t="n">
+      <c r="E78" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
+      <c r="A79" s="4" t="inlineStr">
         <is>
           <t>Nyeri</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B79" s="4" t="inlineStr">
         <is>
           <t>100g</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
+      <c r="C79" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D79" s="4" t="inlineStr">
         <is>
           <t>7.00</t>
         </is>
       </c>
-      <c r="E79" t="n">
+      <c r="E79" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2426,35 +2464,86 @@
         </is>
       </c>
       <c r="E80" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5" t="inlineStr">
+        <is>
+          <t>Nyeri</t>
+        </is>
+      </c>
+      <c r="B81" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C81" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D81" s="5" t="inlineStr">
+        <is>
+          <t>16.30</t>
+        </is>
+      </c>
+      <c r="E81" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5" t="inlineStr">
+        <is>
+          <t>Gyvenimo kava</t>
+        </is>
+      </c>
+      <c r="B82" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C82" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D82" s="5" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="E82" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="inlineStr">
+        <is>
+          <t>Gyvenimo kava</t>
+        </is>
+      </c>
+      <c r="B83" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C83" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D83" s="5" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="E83" s="5" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Nyeri</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>16.30</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add a meaningful error message, write a unit test to test the functionality
</commit_message>
<xml_diff>
--- a/coffee_stock_inventory.xlsx
+++ b/coffee_stock_inventory.xlsx
@@ -618,28 +618,28 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Buna Blend</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>500g</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="E7" s="5" t="n">
-        <v>2</v>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="E9" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -793,28 +793,28 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Koke</t>
         </is>
       </c>
-      <c r="B14" s="5" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D14" s="5" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>15.70</t>
         </is>
       </c>
-      <c r="E14" s="5" t="n">
-        <v>1</v>
+      <c r="E14" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -1014,32 +1014,32 @@
         </is>
       </c>
       <c r="E22" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
+      <c r="A23" s="5" t="inlineStr">
         <is>
           <t>Sidamo</t>
         </is>
       </c>
-      <c r="B23" s="4" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D23" s="4" t="inlineStr">
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
         <is>
           <t>14.00</t>
         </is>
       </c>
-      <c r="E23" s="4" t="n">
-        <v>0</v>
+      <c r="E23" s="5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -1193,28 +1193,28 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="inlineStr">
+      <c r="A30" s="4" t="inlineStr">
         <is>
           <t>Yirgacheffe</t>
         </is>
       </c>
-      <c r="B30" s="5" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C30" s="5" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D30" s="5" t="inlineStr">
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C30" s="4" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
         <is>
           <t>15.70</t>
         </is>
       </c>
-      <c r="E30" s="5" t="n">
-        <v>2</v>
+      <c r="E30" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1914,7 +1914,7 @@
         </is>
       </c>
       <c r="E58" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2143,53 +2143,53 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4" t="inlineStr">
+      <c r="A68" s="5" t="inlineStr">
         <is>
           <t>As ir Tu</t>
         </is>
       </c>
-      <c r="B68" s="4" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C68" s="4" t="inlineStr">
-        <is>
-          <t>Ground</t>
-        </is>
-      </c>
-      <c r="D68" s="4" t="inlineStr">
+      <c r="B68" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C68" s="5" t="inlineStr">
+        <is>
+          <t>Ground</t>
+        </is>
+      </c>
+      <c r="D68" s="5" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E68" s="4" t="n">
-        <v>0</v>
+      <c r="E68" s="5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="4" t="inlineStr">
+      <c r="A69" s="5" t="inlineStr">
         <is>
           <t>As ir Tu</t>
         </is>
       </c>
-      <c r="B69" s="4" t="inlineStr">
-        <is>
-          <t>250g</t>
-        </is>
-      </c>
-      <c r="C69" s="4" t="inlineStr">
-        <is>
-          <t>Beans</t>
-        </is>
-      </c>
-      <c r="D69" s="4" t="inlineStr">
+      <c r="B69" s="5" t="inlineStr">
+        <is>
+          <t>250g</t>
+        </is>
+      </c>
+      <c r="C69" s="5" t="inlineStr">
+        <is>
+          <t>Beans</t>
+        </is>
+      </c>
+      <c r="D69" s="5" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="E69" s="4" t="n">
-        <v>0</v>
+      <c r="E69" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2314,7 +2314,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">

</xml_diff>